<commit_message>
adding more things to the other bot
</commit_message>
<xml_diff>
--- a/scripts/initial_categories.xlsx
+++ b/scripts/initial_categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alon/code/freedom_bot/chatbot/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03D58E2C-5530-4B48-AD8B-27A63EEF60AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B94BC4-4E4E-D94A-BBEE-DE921B3BC979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,12 +28,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>שכר עבודה אריאנה - נטו</t>
-  </si>
-  <si>
-    <t>שכר עבודה אלון - נטו</t>
-  </si>
-  <si>
     <t>הכנסה אחרת / חד פעמית</t>
   </si>
   <si>
@@ -43,9 +37,6 @@
     <t>משכנתא / דמי שכירות</t>
   </si>
   <si>
-    <t>הוצאות תחבורה ציבורית ואופניים</t>
-  </si>
-  <si>
     <t>vital and reoccuring</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
     <t>בייביסיטר</t>
   </si>
   <si>
-    <t>תרופות, בדיקות וטיפולים רפואיים</t>
-  </si>
-  <si>
     <t>vital and changes</t>
   </si>
   <si>
@@ -85,9 +73,6 @@
     <t>סלולארי</t>
   </si>
   <si>
-    <t>מנוי חדר כושר/חוגים</t>
-  </si>
-  <si>
     <t>קורסים</t>
   </si>
   <si>
@@ -97,9 +82,6 @@
     <t>הוצאות רכב</t>
   </si>
   <si>
-    <t>אוכל בחוץ (כולל מסעדות, בתי קפה, משלוחים)</t>
-  </si>
-  <si>
     <t>חניה</t>
   </si>
   <si>
@@ -173,6 +155,24 @@
   </si>
   <si>
     <t>investment</t>
+  </si>
+  <si>
+    <t>רפואה</t>
+  </si>
+  <si>
+    <t>משכורת אריאנה (נטו)</t>
+  </si>
+  <si>
+    <t>משכורת אלון (נטו)</t>
+  </si>
+  <si>
+    <t>תחבורה</t>
+  </si>
+  <si>
+    <t>אוכל בחוץ</t>
+  </si>
+  <si>
+    <t>חדר כושר/חוגים</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1043,338 +1043,338 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved to inine bot
</commit_message>
<xml_diff>
--- a/scripts/initial_categories.xlsx
+++ b/scripts/initial_categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alon/code/freedom_bot/chatbot/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B94BC4-4E4E-D94A-BBEE-DE921B3BC979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC77C28-8206-714B-9F2B-3852A3674C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,24 +136,6 @@
     <t>study</t>
   </si>
   <si>
-    <t>שכירות</t>
-  </si>
-  <si>
-    <t>ביטוח דירה</t>
-  </si>
-  <si>
-    <t>תחזוקה</t>
-  </si>
-  <si>
-    <t>ניהול</t>
-  </si>
-  <si>
-    <t>ריהוט</t>
-  </si>
-  <si>
-    <t>משכנתא</t>
-  </si>
-  <si>
     <t>investment</t>
   </si>
   <si>
@@ -173,6 +155,24 @@
   </si>
   <si>
     <t>חדר כושר/חוגים</t>
+  </si>
+  <si>
+    <t>השקעה - שכירות</t>
+  </si>
+  <si>
+    <t>השקעה - ביטוח דירה</t>
+  </si>
+  <si>
+    <t>השקעה - תחזוקה</t>
+  </si>
+  <si>
+    <t>השקעה - ניהול</t>
+  </si>
+  <si>
+    <t>השקעה - ריהוט</t>
+  </si>
+  <si>
+    <t>השקה - משכנתא</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>35</v>
@@ -1331,50 +1331,50 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed categories to be taken from excel instead of DB. this should make it faster
</commit_message>
<xml_diff>
--- a/scripts/initial_categories.xlsx
+++ b/scripts/initial_categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alon/code/freedom_bot/chatbot/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC77C28-8206-714B-9F2B-3852A3674C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC76C81C-F964-0F4A-A18A-3D4A7CD56813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,7 +172,7 @@
     <t>השקעה - ריהוט</t>
   </si>
   <si>
-    <t>השקה - משכנתא</t>
+    <t>השקעה - משכנתא</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B38" sqref="B37:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>